<commit_message>
Merge updated files from 'main' into production
</commit_message>
<xml_diff>
--- a/public/[Template]-Data-Lowongan.xlsx
+++ b/public/[Template]-Data-Lowongan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_8\Skripji\Skripsi SIG\SIG Kampus Merdeka\Data\Data Clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4462B45-9B89-47C3-BF28-844F8AF9D3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A593F460-68EF-4C5A-8083-0ADE3B2A976B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="90" windowWidth="20445" windowHeight="10710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -64,19 +64,22 @@
     <t>Opportunity 4</t>
   </si>
   <si>
+    <t>Opportunity 5</t>
+  </si>
+  <si>
+    <t>Opportunity 6</t>
+  </si>
+  <si>
+    <t>Opportunity 7</t>
+  </si>
+  <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Pellentesque in mollis nisl, et laoreet arcu. Nam at lectus quis lectus tempor mattis. Sed semper fringilla turpis eu ornare. Pellentesque egestas faucibus feugiat. Nunc finibus est pulvinar diam tempor, quis efficitur metus placerat. Morbi malesuada, est eu fringilla ultrices, turpis risus posuere lorem, ac egestas mauris purus non erat. Fusce congue dui vel justo suscipit, et aliquet elit cursus. Nullam mattis massa malesuada placerat condimentum.</t>
   </si>
   <si>
-    <t>Hybrid</t>
+    <t>2024-05-01T00:00:00.000Z</t>
   </si>
   <si>
-    <t>Opportunity 1</t>
-  </si>
-  <si>
-    <t>Opportunity 2</t>
-  </si>
-  <si>
-    <t>Opportunity 3</t>
+    <t>HYBRID</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,26 +164,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -201,18 +189,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,9 +412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2465"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -470,28 +451,28 @@
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
-      <c r="D2" s="12">
-        <v>45413</v>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>10</v>
@@ -508,22 +489,20 @@
       <c r="I2" s="6">
         <v>1200000</v>
       </c>
-      <c r="J2" s="13">
-        <v>2</v>
+      <c r="J2" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
-        <v>2</v>
+      <c r="A3" s="3"/>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="12">
-        <v>45413</v>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
@@ -540,25 +519,23 @@
       <c r="I3" s="6">
         <v>800000</v>
       </c>
-      <c r="J3" s="14">
-        <v>3</v>
+      <c r="J3" s="13">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
-        <v>3</v>
+      <c r="A4" s="3"/>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="12">
-        <v>45413</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3">
         <v>3</v>
@@ -570,25 +547,25 @@
         <v>0</v>
       </c>
       <c r="I4" s="6"/>
-      <c r="J4" s="13">
-        <v>1</v>
+      <c r="J4" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
-      <c r="D5" s="12">
-        <v>45413</v>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
@@ -600,8 +577,8 @@
         <v>3</v>
       </c>
       <c r="I5" s="8"/>
-      <c r="J5" s="14">
-        <v>3</v>
+      <c r="J5" s="13">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>